<commit_message>
Modification done Select is changed
</commit_message>
<xml_diff>
--- a/src/main/resources/DataObjectsFile.xlsx
+++ b/src/main/resources/DataObjectsFile.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
   <si>
     <t xml:space="preserve">elementName</t>
   </si>
@@ -67,19 +67,25 @@
     <t xml:space="preserve">eightDigitValidation</t>
   </si>
   <si>
+    <t xml:space="preserve">list</t>
+  </si>
+  <si>
+    <t xml:space="preserve">//*[@id=’cfplog__ChangePassword__MiniEightDigit’]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">upperCaseValidation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">select</t>
+  </si>
+  <si>
+    <t xml:space="preserve">//*[@id=’cfplog__ChangePassword__UpperCase’]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lowerCaseValidation</t>
+  </si>
+  <si>
     <t xml:space="preserve">assert</t>
-  </si>
-  <si>
-    <t xml:space="preserve">//*[@id=’cfplog__ChangePassword__MiniEightDigit’]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">upperCaseValidation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">//*[@id=’cfplog__ChangePassword__UpperCase’]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lowerCaseValidation</t>
   </si>
   <si>
     <t xml:space="preserve">//*[@id=’cfplog__ChangePassword__LowerCase’]</t>
@@ -204,7 +210,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="17.35" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -274,7 +280,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="48.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>14</v>
       </c>
@@ -282,6 +288,9 @@
         <v>15</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -290,43 +299,43 @@
         <v>17</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="C9" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Renamed Automator Page Object
</commit_message>
<xml_diff>
--- a/src/main/resources/DataObjectsFile.xlsx
+++ b/src/main/resources/DataObjectsFile.xlsx
@@ -34,13 +34,13 @@
     <t xml:space="preserve">additionalXpath</t>
   </si>
   <si>
-    <t xml:space="preserve">oldPassword</t>
+    <t xml:space="preserve">loginUserName</t>
   </si>
   <si>
     <t xml:space="preserve">text</t>
   </si>
   <si>
-    <t xml:space="preserve">//*[@id=’cfplog__ChangePassword__oldPassword’]</t>
+    <t xml:space="preserve">//*[@id=’cfplog__ChangePassword__username’]</t>
   </si>
   <si>
     <t xml:space="preserve">newPassword</t>
@@ -210,7 +210,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
+      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="17.35" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>